<commit_message>
Comparison with OPS data
</commit_message>
<xml_diff>
--- a/analysis/Comparison_one_region.xlsx
+++ b/analysis/Comparison_one_region.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="23715" windowHeight="9795"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="13">
   <si>
     <t>obj value</t>
   </si>
@@ -30,12 +30,6 @@
     <t>capacities storage GW</t>
   </si>
   <si>
-    <t>Storage costs (our model)</t>
-  </si>
-  <si>
-    <t>Storage costs (Zerrahn &amp; Schill)</t>
-  </si>
-  <si>
     <t>Storage power capacity (Zerrahn &amp; Schill)</t>
   </si>
   <si>
@@ -45,7 +39,22 @@
     <t>Storage power capacity (our model)</t>
   </si>
   <si>
-    <t>Storage energy capacity (our model)</t>
+    <t>Total costs (Zerrahn &amp; Schill)</t>
+  </si>
+  <si>
+    <t>Total costs (our model OPS)</t>
+  </si>
+  <si>
+    <t>Total costs (our model RN)</t>
+  </si>
+  <si>
+    <t>Storage energy capacity (our model  RN)</t>
+  </si>
+  <si>
+    <t>Storage energy capacity (our model  OPS)</t>
+  </si>
+  <si>
+    <t>Storage power capacity (our model  OPS)</t>
   </si>
 </sst>
 </file>
@@ -81,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -110,7 +120,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Storage costs (Zerrahn &amp; Schill)</c:v>
+                  <c:v>Total costs (Zerrahn &amp; Schill)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -177,15 +187,90 @@
           </c:val>
         </c:ser>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total costs (our model OPS)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$M$2:$M$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>26045043473.386299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26796497973.626499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27689450418.857601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28766381236.381199</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30081184989.8759</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31653862952.625999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33418068650.503201</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35428948449.010498</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37704173196.166397</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40297685002.674797</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43370449599.322998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>47102370731.771599</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>51852866886.260597</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>57999068354.8255</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>66421226609.0411</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>79645743258.893005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>138170389719.15201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Tabelle1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Storage costs (our model)</c:v>
+                  <c:v>Total costs (our model RN)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -251,24 +336,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="138088832"/>
-        <c:axId val="138090368"/>
+        <c:axId val="103396480"/>
+        <c:axId val="103398016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="138088832"/>
+        <c:axId val="103396480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138090368"/>
+        <c:crossAx val="103398016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138090368"/>
+        <c:axId val="103398016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -276,7 +361,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138088832"/>
+        <c:crossAx val="103396480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -289,7 +374,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -313,7 +398,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Storage energy capacity (our model)</c:v>
+                  <c:v>Storage energy capacity (our model  RN)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -401,8 +486,59 @@
           </c:val>
         </c:ser>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$N$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Storage energy capacity (our model  OPS)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$O$22:$O$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>22.358754573215201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.115662192671103</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.274111523833099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>131.56112334131399</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>222.406975991948</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>425.39176489940002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>811.98131385889599</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1369.9744642797</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6899.5135992289597</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Tabelle1!$E$31</c:f>
@@ -416,10 +552,10 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$E$32:$E$39</c:f>
+              <c:f>Tabelle1!$E$32:$E$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>3.2001532511485502</c:v>
                 </c:pt>
@@ -443,14 +579,17 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>46.023171680210197</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>79.5757548765542</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Tabelle1!$J$31</c:f>
@@ -464,10 +603,10 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$J$32:$J$39</c:f>
+              <c:f>Tabelle1!$J$32:$J$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>13.730586942885701</c:v>
                 </c:pt>
@@ -491,29 +630,83 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>66.012191456894001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72.395574881031393</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="94801920"/>
-        <c:axId val="94803456"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$N$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Storage power capacity (our model  OPS)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$O$32:$O$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.0860545692324202</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8841990168398404</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.1201090451374398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.5408606681814</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.432980433659701</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.225243678634399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.557895008342001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48.376344337157903</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78.9941925587123</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="103444864"/>
+        <c:axId val="103446400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="94801920"/>
+        <c:axId val="103444864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94803456"/>
+        <c:crossAx val="103446400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94803456"/>
+        <c:axId val="103446400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -521,7 +714,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94801920"/>
+        <c:crossAx val="103444864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -534,7 +727,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -544,16 +737,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>485774</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>447674</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -574,16 +767,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>428623</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>523873</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -890,23 +1083,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" topLeftCell="I9" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:13">
       <c r="D1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -931,8 +1127,23 @@
       <c r="H2">
         <v>25043771028.400398</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
+      </c>
+      <c r="L2">
+        <v>1000</v>
+      </c>
+      <c r="M2">
+        <v>26045043473.386299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -957,8 +1168,23 @@
       <c r="H3">
         <v>25548702210.486599</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>25</v>
+      </c>
+      <c r="L3">
+        <v>1000</v>
+      </c>
+      <c r="M3">
+        <v>26796497973.626499</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -983,8 +1209,23 @@
       <c r="H4">
         <v>26141351085.510601</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>30</v>
+      </c>
+      <c r="L4">
+        <v>1000</v>
+      </c>
+      <c r="M4">
+        <v>27689450418.857601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1009,8 +1250,23 @@
       <c r="H5">
         <v>26895463175.052601</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>35</v>
+      </c>
+      <c r="L5">
+        <v>1000</v>
+      </c>
+      <c r="M5">
+        <v>28766381236.381199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1035,8 +1291,23 @@
       <c r="H6">
         <v>27794879997.733002</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>40</v>
+      </c>
+      <c r="L6">
+        <v>1000</v>
+      </c>
+      <c r="M6">
+        <v>30081184989.8759</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1061,8 +1332,23 @@
       <c r="H7">
         <v>28864085566.101002</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>45</v>
+      </c>
+      <c r="L7">
+        <v>1000</v>
+      </c>
+      <c r="M7">
+        <v>31653862952.625999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1087,8 +1373,23 @@
       <c r="H8">
         <v>30115678119.164501</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>50</v>
+      </c>
+      <c r="L8">
+        <v>1000</v>
+      </c>
+      <c r="M8">
+        <v>33418068650.503201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1113,8 +1414,23 @@
       <c r="H9">
         <v>31546752626.7131</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>55</v>
+      </c>
+      <c r="L9">
+        <v>1000</v>
+      </c>
+      <c r="M9">
+        <v>35428948449.010498</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1139,8 +1455,23 @@
       <c r="H10">
         <v>33197530111.720501</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>60</v>
+      </c>
+      <c r="L10">
+        <v>1000</v>
+      </c>
+      <c r="M10">
+        <v>37704173196.166397</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1165,8 +1496,23 @@
       <c r="H11">
         <v>35089993878.859299</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>65</v>
+      </c>
+      <c r="L11">
+        <v>1000</v>
+      </c>
+      <c r="M11">
+        <v>40297685002.674797</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1191,8 +1537,23 @@
       <c r="H12">
         <v>37320129213.218102</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>70</v>
+      </c>
+      <c r="L12">
+        <v>1000</v>
+      </c>
+      <c r="M12">
+        <v>43370449599.322998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1217,8 +1578,23 @@
       <c r="H13">
         <v>40069984654.877998</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>75</v>
+      </c>
+      <c r="L13">
+        <v>1000</v>
+      </c>
+      <c r="M13">
+        <v>47102370731.771599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1243,8 +1619,23 @@
       <c r="H14">
         <v>43585850853.940201</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>80</v>
+      </c>
+      <c r="L14">
+        <v>1000</v>
+      </c>
+      <c r="M14">
+        <v>51852866886.260597</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1269,8 +1660,23 @@
       <c r="H15">
         <v>48258005810.402901</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>85</v>
+      </c>
+      <c r="L15">
+        <v>1000</v>
+      </c>
+      <c r="M15">
+        <v>57999068354.8255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1295,8 +1701,23 @@
       <c r="H16">
         <v>54753680840.938904</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>90</v>
+      </c>
+      <c r="L16">
+        <v>1000</v>
+      </c>
+      <c r="M16">
+        <v>66421226609.0411</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1321,8 +1742,23 @@
       <c r="H17">
         <v>64767845285.3162</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="I17" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>95</v>
+      </c>
+      <c r="L17">
+        <v>1000</v>
+      </c>
+      <c r="M17">
+        <v>79645743258.893005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1347,16 +1783,37 @@
       <c r="H18">
         <v>106008937642.51199</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="I18" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>100</v>
+      </c>
+      <c r="L18">
+        <v>1000</v>
+      </c>
+      <c r="M18">
+        <v>138170389719.15201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15">
       <c r="E21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>5</v>
+      </c>
+      <c r="N21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1387,8 +1844,23 @@
       <c r="J22">
         <v>108.110683646879</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>60</v>
+      </c>
+      <c r="M22">
+        <v>1000</v>
+      </c>
+      <c r="N22" t="s">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>22.358754573215201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1419,8 +1891,23 @@
       <c r="J23">
         <v>176.41904248464601</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>65</v>
+      </c>
+      <c r="M23">
+        <v>1000</v>
+      </c>
+      <c r="N23" t="s">
+        <v>2</v>
+      </c>
+      <c r="O23">
+        <v>44.115662192671103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1451,8 +1938,23 @@
       <c r="J24">
         <v>230.30435560974399</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24" t="s">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>70</v>
+      </c>
+      <c r="M24">
+        <v>1000</v>
+      </c>
+      <c r="N24" t="s">
+        <v>2</v>
+      </c>
+      <c r="O24">
+        <v>74.274111523833099</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1483,8 +1985,23 @@
       <c r="J25">
         <v>314.19776332554699</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25" t="s">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>75</v>
+      </c>
+      <c r="M25">
+        <v>1000</v>
+      </c>
+      <c r="N25" t="s">
+        <v>2</v>
+      </c>
+      <c r="O25">
+        <v>131.56112334131399</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1515,8 +2032,23 @@
       <c r="J26">
         <v>461.943161699933</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26" t="s">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>80</v>
+      </c>
+      <c r="M26">
+        <v>1000</v>
+      </c>
+      <c r="N26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O26">
+        <v>222.406975991948</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -1547,8 +2079,23 @@
       <c r="J27">
         <v>692.91434196559601</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27" t="s">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>85</v>
+      </c>
+      <c r="M27">
+        <v>1000</v>
+      </c>
+      <c r="N27" t="s">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>425.39176489940002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1579,8 +2126,23 @@
       <c r="J28">
         <v>1076.9326465787201</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28" t="s">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>90</v>
+      </c>
+      <c r="M28">
+        <v>1000</v>
+      </c>
+      <c r="N28" t="s">
+        <v>2</v>
+      </c>
+      <c r="O28">
+        <v>811.98131385889599</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1611,8 +2173,23 @@
       <c r="J29">
         <v>1633.64267479667</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29" t="s">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>95</v>
+      </c>
+      <c r="M29">
+        <v>1000</v>
+      </c>
+      <c r="N29" t="s">
+        <v>2</v>
+      </c>
+      <c r="O29">
+        <v>1369.9744642797</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1643,16 +2220,34 @@
       <c r="J30">
         <v>5635.9607822053304</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30" t="s">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>100</v>
+      </c>
+      <c r="M30">
+        <v>1000</v>
+      </c>
+      <c r="N30" t="s">
+        <v>2</v>
+      </c>
+      <c r="O30">
+        <v>6899.5135992289597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="E31" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="N31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1683,8 +2278,23 @@
       <c r="J32">
         <v>13.730586942885701</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32" t="s">
+        <v>3</v>
+      </c>
+      <c r="L32">
+        <v>60</v>
+      </c>
+      <c r="M32">
+        <v>1000</v>
+      </c>
+      <c r="N32" t="s">
+        <v>2</v>
+      </c>
+      <c r="O32">
+        <v>4.0860545692324202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1715,8 +2325,23 @@
       <c r="J33">
         <v>21.6866062055309</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33" t="s">
+        <v>3</v>
+      </c>
+      <c r="L33">
+        <v>65</v>
+      </c>
+      <c r="M33">
+        <v>1000</v>
+      </c>
+      <c r="N33" t="s">
+        <v>2</v>
+      </c>
+      <c r="O33">
+        <v>5.8841990168398404</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -1747,8 +2372,23 @@
       <c r="J34">
         <v>29.291141532540301</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34" t="s">
+        <v>3</v>
+      </c>
+      <c r="L34">
+        <v>70</v>
+      </c>
+      <c r="M34">
+        <v>1000</v>
+      </c>
+      <c r="N34" t="s">
+        <v>2</v>
+      </c>
+      <c r="O34">
+        <v>8.1201090451374398</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -1779,8 +2419,23 @@
       <c r="J35">
         <v>37.322316688473201</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35" t="s">
+        <v>3</v>
+      </c>
+      <c r="L35">
+        <v>75</v>
+      </c>
+      <c r="M35">
+        <v>1000</v>
+      </c>
+      <c r="N35" t="s">
+        <v>2</v>
+      </c>
+      <c r="O35">
+        <v>11.5408606681814</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -1811,8 +2466,23 @@
       <c r="J36">
         <v>45.820131677486899</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="K36" t="s">
+        <v>3</v>
+      </c>
+      <c r="L36">
+        <v>80</v>
+      </c>
+      <c r="M36">
+        <v>1000</v>
+      </c>
+      <c r="N36" t="s">
+        <v>2</v>
+      </c>
+      <c r="O36">
+        <v>16.432980433659701</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -1843,8 +2513,23 @@
       <c r="J37">
         <v>51.859443287387002</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37" t="s">
+        <v>3</v>
+      </c>
+      <c r="L37">
+        <v>85</v>
+      </c>
+      <c r="M37">
+        <v>1000</v>
+      </c>
+      <c r="N37" t="s">
+        <v>2</v>
+      </c>
+      <c r="O37">
+        <v>24.225243678634399</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1875,8 +2560,23 @@
       <c r="J38">
         <v>58.162749772688102</v>
       </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="K38" t="s">
+        <v>3</v>
+      </c>
+      <c r="L38">
+        <v>90</v>
+      </c>
+      <c r="M38">
+        <v>1000</v>
+      </c>
+      <c r="N38" t="s">
+        <v>2</v>
+      </c>
+      <c r="O38">
+        <v>33.557895008342001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1907,8 +2607,23 @@
       <c r="J39">
         <v>66.012191456894001</v>
       </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="K39" t="s">
+        <v>3</v>
+      </c>
+      <c r="L39">
+        <v>95</v>
+      </c>
+      <c r="M39">
+        <v>1000</v>
+      </c>
+      <c r="N39" t="s">
+        <v>2</v>
+      </c>
+      <c r="O39">
+        <v>48.376344337157903</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -1938,6 +2653,21 @@
       </c>
       <c r="J40">
         <v>72.395574881031393</v>
+      </c>
+      <c r="K40" t="s">
+        <v>3</v>
+      </c>
+      <c r="L40">
+        <v>100</v>
+      </c>
+      <c r="M40">
+        <v>1000</v>
+      </c>
+      <c r="N40" t="s">
+        <v>2</v>
+      </c>
+      <c r="O40">
+        <v>78.9941925587123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split up original model for comparison
</commit_message>
<xml_diff>
--- a/analysis/Comparison_one_region.xlsx
+++ b/analysis/Comparison_one_region.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="23715" windowHeight="9795" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="23715" windowHeight="9795"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="36">
   <si>
     <t>obj value</t>
   </si>
@@ -71,12 +71,69 @@
   <si>
     <t>Our Model Version 2: OPSD Data</t>
   </si>
+  <si>
+    <t>Schill and Zerrahn: Two regions and RN data</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -138,6 +195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -159,28 +217,91 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Schill and Zerrahn: Two regions and RN data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$S$4:$S$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>25630273922.891468</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26251919628.188221</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26917927409.760231</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27626498076.651402</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28411140381.213257</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29324902278.857162</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30383069835.099846</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31676009981.071243</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33256157070.672783</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35194581475.868912</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37538553082.631386</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40402253011.706009</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43978913257.62439</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>48691343979.105606</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>55112691834.013161</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>65111313475.25174</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>104539453646.40437</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Tabelle1!$A$1</c:f>
@@ -192,7 +313,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Tabelle1!$D$4:$D$20</c:f>
@@ -256,7 +376,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Tabelle1!$L$1</c:f>
@@ -268,7 +388,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Tabelle1!$O$4:$O$20</c:f>
@@ -332,7 +451,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Tabelle1!$F$1</c:f>
@@ -344,7 +463,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Tabelle1!$I$4:$I$20</c:f>
@@ -406,48 +524,33 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="52859264"/>
-        <c:axId val="52860800"/>
+        <c:dLbls/>
+        <c:axId val="51245824"/>
+        <c:axId val="51247360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52859264"/>
+        <c:axId val="51245824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52860800"/>
+        <c:crossAx val="51247360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52860800"/>
+        <c:axId val="51247360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52859264"/>
+        <c:crossAx val="51245824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -455,15 +558,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -471,24 +572,12 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -563,7 +652,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -639,7 +727,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -715,7 +802,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -791,67 +877,48 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="118375168"/>
-        <c:axId val="118376704"/>
+        <c:axId val="51562368"/>
+        <c:axId val="51563904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="118375168"/>
+        <c:axId val="51562368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118376704"/>
+        <c:crossAx val="51563904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118376704"/>
+        <c:axId val="51563904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118375168"/>
+        <c:crossAx val="51562368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -867,10 +934,10 @@
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>57978</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>124239</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -928,7 +995,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -1002,7 +1069,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1037,7 +1103,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1213,14 +1278,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView tabSelected="1" topLeftCell="L37" workbookViewId="0">
+      <selection activeCell="S52" sqref="S52:S85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
@@ -1235,7 +1300,7 @@
     <col min="16" max="16" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -1245,8 +1310,11 @@
       <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1254,7 +1322,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1291,8 +1359,17 @@
       <c r="O4" s="4">
         <v>27377431082.9832</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4">
+        <v>25630273922.891468</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1329,8 +1406,17 @@
       <c r="O5" s="4">
         <v>28407417449.820599</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5">
+        <v>26251919628.188221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1367,8 +1453,17 @@
       <c r="O6" s="4">
         <v>29460934386.633598</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6">
+        <v>26917927409.760231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1405,8 +1500,17 @@
       <c r="O7" s="4">
         <v>30567557106.348</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="S7">
+        <v>27626498076.651402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1443,8 +1547,17 @@
       <c r="O8" s="4">
         <v>31790709659.260601</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8">
+        <v>28411140381.213257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1481,8 +1594,17 @@
       <c r="O9" s="4">
         <v>33163409563.269001</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9">
+        <v>29324902278.857162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1519,8 +1641,17 @@
       <c r="O10" s="4">
         <v>34729548778.942902</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="S10">
+        <v>30383069835.099846</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1557,8 +1688,17 @@
       <c r="O11" s="4">
         <v>36587258765.467796</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S11">
+        <v>31676009981.071243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1595,8 +1735,17 @@
       <c r="O12" s="4">
         <v>38785819245.567902</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S12">
+        <v>33256157070.672783</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1633,8 +1782,17 @@
       <c r="O13" s="4">
         <v>41240406484.9841</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13">
+        <v>35194581475.868912</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1671,8 +1829,17 @@
       <c r="O14" s="4">
         <v>43963183315.678703</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14">
+        <v>37538553082.631386</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1709,8 +1876,17 @@
       <c r="O15" s="4">
         <v>47042941147.296799</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="S15">
+        <v>40402253011.706009</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1747,8 +1923,17 @@
       <c r="O16" s="4">
         <v>50583574564.091797</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="S16">
+        <v>43978913257.62439</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1785,8 +1970,17 @@
       <c r="O17" s="4">
         <v>54806005624.891998</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S17">
+        <v>48691343979.105606</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1823,8 +2017,17 @@
       <c r="O18" s="4">
         <v>60438128960.913597</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S18">
+        <v>55112691834.013161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1861,8 +2064,17 @@
       <c r="O19" s="4">
         <v>69918078241.133698</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="S19">
+        <v>65111313475.25174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1899,17 +2111,26 @@
       <c r="O20" s="4">
         <v>102741666750.116</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S20">
+        <v>104539453646.40437</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20">
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20">
       <c r="O24" s="4"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1946,8 +2167,20 @@
       <c r="O25">
         <v>8.3235041851024096</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S25" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T25">
+        <v>3.9363137556448589</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1984,8 +2217,20 @@
       <c r="O26">
         <v>18.1213844641184</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="S26" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T26">
+        <v>15.640046305195561</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27" s="5" t="s">
         <v>1</v>
       </c>
@@ -2022,8 +2267,20 @@
       <c r="O27">
         <v>34.943852431275801</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q27" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R27" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T27">
+        <v>27.911328960919867</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
       <c r="A28" s="5" t="s">
         <v>1</v>
       </c>
@@ -2060,8 +2317,20 @@
       <c r="O28">
         <v>53.700259094183203</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q28" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R28" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S28" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T28">
+        <v>45.173932317215353</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
       <c r="A29" s="5" t="s">
         <v>1</v>
       </c>
@@ -2098,8 +2367,20 @@
       <c r="O29">
         <v>108.110683646879</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S29" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T29">
+        <v>66.429751223775057</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -2136,8 +2417,20 @@
       <c r="O30">
         <v>176.41904248464601</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q30" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R30" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S30" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T30">
+        <v>108.44498041714959</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
       <c r="A31" s="5" t="s">
         <v>1</v>
       </c>
@@ -2174,8 +2467,20 @@
       <c r="O31">
         <v>230.30435560974399</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="S31" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T31">
+        <v>168.11415311365604</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
       <c r="A32" s="5" t="s">
         <v>1</v>
       </c>
@@ -2212,8 +2517,20 @@
       <c r="O32">
         <v>314.19776332554699</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q32" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="S32" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T32">
+        <v>271.4290211771247</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
       <c r="A33" s="5" t="s">
         <v>1</v>
       </c>
@@ -2250,8 +2567,20 @@
       <c r="O33">
         <v>461.943161699933</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q33" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R33" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S33" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T33">
+        <v>434.8483357333443</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
       <c r="A34" s="5" t="s">
         <v>1</v>
       </c>
@@ -2288,8 +2617,20 @@
       <c r="O34">
         <v>692.91434196559601</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q34" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R34" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S34" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T34">
+        <v>777.42146498197337</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20">
       <c r="A35" s="5" t="s">
         <v>1</v>
       </c>
@@ -2326,8 +2667,20 @@
       <c r="O35">
         <v>1076.9326465787201</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q35" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R35" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="S35" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T35">
+        <v>1630.0348994613566</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20">
       <c r="A36" s="5" t="s">
         <v>1</v>
       </c>
@@ -2364,8 +2717,20 @@
       <c r="O36">
         <v>1633.64267479667</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q36" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R36" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S36" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T36">
+        <v>3253.125501678649</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20">
       <c r="A37" s="5" t="s">
         <v>3</v>
       </c>
@@ -2402,8 +2767,20 @@
       <c r="O37">
         <v>5635.9607822053304</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q37" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R37" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S37" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T37">
+        <v>1.2149116529768083</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -2440,8 +2817,20 @@
       <c r="O38">
         <v>2.80593404651384</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q38" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R38" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="S38" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T38">
+        <v>3.5403327857140066</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -2478,8 +2867,20 @@
       <c r="O39">
         <v>4.7536660352939304</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q39" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R39" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S39" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T39">
+        <v>4.9226329737072057</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -2516,8 +2917,20 @@
       <c r="O40">
         <v>6.1629369367329403</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q40" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R40" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S40" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T40">
+        <v>6.3377290671085946</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -2554,8 +2967,20 @@
       <c r="O41">
         <v>7.5268111117169996</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q41" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T41">
+        <v>7.9134167885288038</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -2592,8 +3017,20 @@
       <c r="O42">
         <v>13.730586942885701</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q42" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R42" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S42" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T42">
+        <v>10.995846945178403</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -2630,8 +3067,20 @@
       <c r="O43">
         <v>21.6866062055309</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q43" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R43" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="S43" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T43">
+        <v>14.675460468776755</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -2668,8 +3117,20 @@
       <c r="O44">
         <v>29.291141532540301</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q44" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R44" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="S44" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T44">
+        <v>19.593967915324392</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -2706,8 +3167,20 @@
       <c r="O45">
         <v>37.322316688473201</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q45" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R45" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S45" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T45">
+        <v>26.407884257261699</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -2744,8 +3217,20 @@
       <c r="O46">
         <v>45.820131677486899</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q46" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R46" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S46" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T46">
+        <v>35.491496655314492</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -2782,8 +3267,20 @@
       <c r="O47">
         <v>51.859443287387002</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q47" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R47" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="S47" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T47">
+        <v>47.563064281238724</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -2820,8 +3317,20 @@
       <c r="O48">
         <v>58.162749772688102</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q48" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R48" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S48" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T48">
+        <v>90.027276665911714</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20">
       <c r="L49" t="s">
         <v>3</v>
       </c>
@@ -2835,7 +3344,7 @@
         <v>66.012191456894001</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20">
       <c r="L50" t="s">
         <v>3</v>
       </c>
@@ -2849,7 +3358,7 @@
         <v>72.395574881031393</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -2886,8 +3395,20 @@
       <c r="O52">
         <v>84.657409083336105</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q52" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R52" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="S52" t="s">
+        <v>5</v>
+      </c>
+      <c r="T52">
+        <v>10.48541840121662</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -2924,8 +3445,20 @@
       <c r="O53">
         <v>105.829334442812</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q53" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R53" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S53" t="s">
+        <v>5</v>
+      </c>
+      <c r="T53">
+        <v>21.273679630348287</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -2962,8 +3495,20 @@
       <c r="O54">
         <v>127.178159851809</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q54" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R54" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="S54" t="s">
+        <v>5</v>
+      </c>
+      <c r="T54">
+        <v>34.474052308688236</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -3000,8 +3545,20 @@
       <c r="O55">
         <v>149.07223229163299</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q55" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R55" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="S55" t="s">
+        <v>5</v>
+      </c>
+      <c r="T55">
+        <v>49.07233100395684</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -3038,8 +3595,20 @@
       <c r="O56">
         <v>172.36182178987701</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R56" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S56" t="s">
+        <v>5</v>
+      </c>
+      <c r="T56">
+        <v>62.708387668816904</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -3076,8 +3645,20 @@
       <c r="O57">
         <v>197.046526564798</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q57" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R57" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S57" t="s">
+        <v>5</v>
+      </c>
+      <c r="T57">
+        <v>75.355041276278996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -3114,8 +3695,20 @@
       <c r="O58">
         <v>223.45507303514</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q58" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R58" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="S58" t="s">
+        <v>5</v>
+      </c>
+      <c r="T58">
+        <v>87.771385262334604</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -3152,8 +3745,20 @@
       <c r="O59">
         <v>252.91582831805999</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q59" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R59" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S59" t="s">
+        <v>5</v>
+      </c>
+      <c r="T59">
+        <v>103.28995020855777</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -3190,8 +3795,20 @@
       <c r="O60">
         <v>282.57138803276501</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q60" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R60" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S60" t="s">
+        <v>5</v>
+      </c>
+      <c r="T60">
+        <v>121.36400292294937</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -3228,8 +3845,20 @@
       <c r="O61">
         <v>313.26483723789602</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q61" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R61" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S61" t="s">
+        <v>5</v>
+      </c>
+      <c r="T61">
+        <v>142.72472818322404</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -3266,8 +3895,20 @@
       <c r="O62">
         <v>345.65635323478199</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q62" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R62" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S62" t="s">
+        <v>5</v>
+      </c>
+      <c r="T62">
+        <v>165.43808632056721</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -3304,8 +3945,20 @@
       <c r="O63">
         <v>381.97531203972102</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q63" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R63" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="S63" t="s">
+        <v>5</v>
+      </c>
+      <c r="T63">
+        <v>190.99042036814745</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -3342,8 +3995,20 @@
       <c r="O64">
         <v>420.24180759976201</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q64" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R64" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="S64" t="s">
+        <v>5</v>
+      </c>
+      <c r="T64">
+        <v>219.34694327276196</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -3380,8 +4045,20 @@
       <c r="O65">
         <v>463.32130696954698</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q65" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R65" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S65" t="s">
+        <v>5</v>
+      </c>
+      <c r="T65">
+        <v>251.98509691541216</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -3418,8 +4095,20 @@
       <c r="O66">
         <v>514.613847064781</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q66" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R66" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S66" t="s">
+        <v>5</v>
+      </c>
+      <c r="T66">
+        <v>287.90085911911973</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -3456,8 +4145,20 @@
       <c r="O67">
         <v>600.29164139147497</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q67" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R67" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="S67" t="s">
+        <v>5</v>
+      </c>
+      <c r="T67">
+        <v>330.61069941039653</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -3494,8 +4195,20 @@
       <c r="O68">
         <v>760.36856534987703</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q68" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R68" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S68" t="s">
+        <v>5</v>
+      </c>
+      <c r="T68">
+        <v>495.32813191642441</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
       <c r="A69" t="s">
         <v>4</v>
       </c>
@@ -3520,8 +4233,20 @@
       <c r="I69">
         <v>151.777571982533</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q69" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R69" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="S69" t="s">
+        <v>6</v>
+      </c>
+      <c r="T69">
+        <v>75.866551990794704</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -3546,8 +4271,20 @@
       <c r="I70">
         <v>149.23084252307299</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q70" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R70" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S70" t="s">
+        <v>6</v>
+      </c>
+      <c r="T70">
+        <v>82.2807517404202</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20">
       <c r="A71" t="s">
         <v>4</v>
       </c>
@@ -3572,8 +4309,20 @@
       <c r="I71">
         <v>176.17731352102999</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q71" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R71" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="S71" t="s">
+        <v>6</v>
+      </c>
+      <c r="T71">
+        <v>85.167920496918939</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20">
       <c r="A72" t="s">
         <v>4</v>
       </c>
@@ -3598,8 +4347,20 @@
       <c r="I72">
         <v>162.66654758016099</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q72" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R72" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="S72" t="s">
+        <v>6</v>
+      </c>
+      <c r="T72">
+        <v>86.174999465670624</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20">
       <c r="A73" t="s">
         <v>4</v>
       </c>
@@ -3624,8 +4385,20 @@
       <c r="I73">
         <v>203.415304461349</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q73" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R73" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S73" t="s">
+        <v>6</v>
+      </c>
+      <c r="T73">
+        <v>89.763559771025925</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20">
       <c r="A74" t="s">
         <v>4</v>
       </c>
@@ -3650,8 +4423,20 @@
       <c r="I74">
         <v>177.79763146124199</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q74" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R74" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S74" t="s">
+        <v>6</v>
+      </c>
+      <c r="T74">
+        <v>96.641522921845208</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20">
       <c r="A75" t="s">
         <v>4</v>
       </c>
@@ -3676,8 +4461,20 @@
       <c r="I75">
         <v>236.841262015041</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q75" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R75" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="S75" t="s">
+        <v>6</v>
+      </c>
+      <c r="T75">
+        <v>105.65317380546698</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20">
       <c r="A76" t="s">
         <v>4</v>
       </c>
@@ -3702,8 +4499,20 @@
       <c r="I76">
         <v>197.32606389790101</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q76" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R76" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S76" t="s">
+        <v>6</v>
+      </c>
+      <c r="T76">
+        <v>112.79150030920896</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20">
       <c r="A77" t="s">
         <v>4</v>
       </c>
@@ -3728,8 +4537,20 @@
       <c r="I77">
         <v>273.10456344717102</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q77" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R77" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S77" t="s">
+        <v>6</v>
+      </c>
+      <c r="T77">
+        <v>119.80669978917342</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20">
       <c r="A78" t="s">
         <v>4</v>
       </c>
@@ -3754,8 +4575,20 @@
       <c r="I78">
         <v>221.12393511492499</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q78" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S78" t="s">
+        <v>6</v>
+      </c>
+      <c r="T78">
+        <v>126.58572236929406</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20">
       <c r="A79" t="s">
         <v>4</v>
       </c>
@@ -3780,8 +4613,20 @@
       <c r="I79">
         <v>317.49778655421699</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q79" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R79" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S79" t="s">
+        <v>6</v>
+      </c>
+      <c r="T79">
+        <v>135.56876011561096</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20">
       <c r="A80" t="s">
         <v>4</v>
       </c>
@@ -3806,8 +4651,20 @@
       <c r="I80">
         <v>255.69469991931999</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q80" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R80" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="S80" t="s">
+        <v>6</v>
+      </c>
+      <c r="T80">
+        <v>146.67988845675583</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20">
       <c r="A81" t="s">
         <v>4</v>
       </c>
@@ -3832,8 +4689,20 @@
       <c r="I81">
         <v>362.342747111682</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q81" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R81" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="S81" t="s">
+        <v>6</v>
+      </c>
+      <c r="T81">
+        <v>161.42484133899987</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20">
       <c r="A82" t="s">
         <v>4</v>
       </c>
@@ -3858,8 +4727,20 @@
       <c r="I82">
         <v>304.998997679887</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q82" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R82" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="S82" t="s">
+        <v>6</v>
+      </c>
+      <c r="T82">
+        <v>182.19762201709713</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20">
       <c r="A83" t="s">
         <v>4</v>
       </c>
@@ -3884,8 +4765,20 @@
       <c r="I83">
         <v>444.16517055655299</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q83" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R83" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S83" t="s">
+        <v>6</v>
+      </c>
+      <c r="T83">
+        <v>209.16940749669939</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20">
       <c r="A84" t="s">
         <v>4</v>
       </c>
@@ -3910,8 +4803,20 @@
       <c r="I84">
         <v>526.86230603096601</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q84" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R84" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="S84" t="s">
+        <v>6</v>
+      </c>
+      <c r="T84">
+        <v>240.69591063023179</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20">
       <c r="A85" t="s">
         <v>4</v>
       </c>
@@ -3936,6 +4841,368 @@
       <c r="I85">
         <v>569.31523837859095</v>
       </c>
+      <c r="Q85" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R85" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S85" t="s">
+        <v>6</v>
+      </c>
+      <c r="T85">
+        <v>468.39848449612236</v>
+      </c>
+    </row>
+    <row r="100" spans="19:21">
+      <c r="S100" s="8"/>
+      <c r="T100" s="8"/>
+      <c r="U100" s="8"/>
+    </row>
+    <row r="101" spans="19:21">
+      <c r="S101" s="8"/>
+      <c r="T101" s="8"/>
+      <c r="U101" s="8"/>
+    </row>
+    <row r="102" spans="19:21">
+      <c r="S102" s="8"/>
+      <c r="T102" s="8"/>
+      <c r="U102" s="8"/>
+    </row>
+    <row r="103" spans="19:21">
+      <c r="S103" s="8"/>
+      <c r="T103" s="8"/>
+      <c r="U103" s="8"/>
+    </row>
+    <row r="104" spans="19:21">
+      <c r="S104" s="8"/>
+      <c r="T104" s="8"/>
+      <c r="U104" s="8"/>
+    </row>
+    <row r="105" spans="19:21">
+      <c r="S105" s="8"/>
+      <c r="T105" s="8"/>
+      <c r="U105" s="8"/>
+    </row>
+    <row r="106" spans="19:21">
+      <c r="S106" s="8"/>
+      <c r="T106" s="8"/>
+      <c r="U106" s="8"/>
+    </row>
+    <row r="107" spans="19:21">
+      <c r="S107" s="8"/>
+      <c r="T107" s="8"/>
+      <c r="U107" s="8"/>
+    </row>
+    <row r="108" spans="19:21">
+      <c r="S108" s="8"/>
+      <c r="T108" s="8"/>
+      <c r="U108" s="8"/>
+    </row>
+    <row r="109" spans="19:21">
+      <c r="S109" s="8"/>
+      <c r="T109" s="8"/>
+      <c r="U109" s="8"/>
+    </row>
+    <row r="110" spans="19:21">
+      <c r="S110" s="8"/>
+      <c r="T110" s="8"/>
+      <c r="U110" s="8"/>
+    </row>
+    <row r="111" spans="19:21">
+      <c r="S111" s="8"/>
+      <c r="T111" s="8"/>
+      <c r="U111" s="8"/>
+    </row>
+    <row r="112" spans="19:21">
+      <c r="S112" s="8"/>
+      <c r="T112" s="8"/>
+      <c r="U112" s="8"/>
+    </row>
+    <row r="113" spans="19:21">
+      <c r="S113" s="8"/>
+      <c r="T113" s="8"/>
+      <c r="U113" s="8"/>
+    </row>
+    <row r="114" spans="19:21">
+      <c r="S114" s="8"/>
+      <c r="T114" s="8"/>
+      <c r="U114" s="8"/>
+    </row>
+    <row r="115" spans="19:21">
+      <c r="S115" s="8"/>
+      <c r="T115" s="8"/>
+      <c r="U115" s="8"/>
+    </row>
+    <row r="116" spans="19:21">
+      <c r="S116" s="8"/>
+      <c r="T116" s="8"/>
+      <c r="U116" s="8"/>
+    </row>
+    <row r="117" spans="19:21">
+      <c r="S117" s="8"/>
+      <c r="T117" s="8"/>
+      <c r="U117" s="8"/>
+    </row>
+    <row r="181" spans="21:23">
+      <c r="U181" s="8"/>
+      <c r="V181" s="8"/>
+      <c r="W181" s="8"/>
+    </row>
+    <row r="182" spans="21:23">
+      <c r="U182" s="8"/>
+      <c r="V182" s="8"/>
+      <c r="W182" s="8"/>
+    </row>
+    <row r="183" spans="21:23">
+      <c r="U183" s="8"/>
+      <c r="V183" s="8"/>
+      <c r="W183" s="8"/>
+    </row>
+    <row r="184" spans="21:23">
+      <c r="U184" s="8"/>
+      <c r="V184" s="8"/>
+      <c r="W184" s="8"/>
+    </row>
+    <row r="185" spans="21:23">
+      <c r="U185" s="8"/>
+      <c r="V185" s="8"/>
+      <c r="W185" s="8"/>
+    </row>
+    <row r="186" spans="21:23">
+      <c r="U186" s="8"/>
+      <c r="V186" s="8"/>
+      <c r="W186" s="8"/>
+    </row>
+    <row r="187" spans="21:23">
+      <c r="U187" s="8"/>
+      <c r="V187" s="8"/>
+      <c r="W187" s="8"/>
+    </row>
+    <row r="188" spans="21:23">
+      <c r="U188" s="8"/>
+      <c r="V188" s="8"/>
+      <c r="W188" s="8"/>
+    </row>
+    <row r="189" spans="21:23">
+      <c r="U189" s="8"/>
+      <c r="V189" s="8"/>
+      <c r="W189" s="8"/>
+    </row>
+    <row r="190" spans="21:23">
+      <c r="U190" s="8"/>
+      <c r="V190" s="8"/>
+      <c r="W190" s="8"/>
+    </row>
+    <row r="191" spans="21:23">
+      <c r="U191" s="8"/>
+      <c r="V191" s="8"/>
+      <c r="W191" s="8"/>
+    </row>
+    <row r="192" spans="21:23">
+      <c r="U192" s="8"/>
+      <c r="V192" s="8"/>
+      <c r="W192" s="8"/>
+    </row>
+    <row r="193" spans="21:23">
+      <c r="U193" s="8"/>
+      <c r="V193" s="8"/>
+      <c r="W193" s="8"/>
+    </row>
+    <row r="194" spans="21:23">
+      <c r="U194" s="8"/>
+      <c r="V194" s="8"/>
+      <c r="W194" s="8"/>
+    </row>
+    <row r="195" spans="21:23">
+      <c r="U195" s="8"/>
+      <c r="V195" s="8"/>
+      <c r="W195" s="8"/>
+    </row>
+    <row r="196" spans="21:23">
+      <c r="U196" s="8"/>
+      <c r="V196" s="8"/>
+      <c r="W196" s="8"/>
+    </row>
+    <row r="197" spans="21:23">
+      <c r="U197" s="8"/>
+      <c r="V197" s="8"/>
+      <c r="W197" s="8"/>
+    </row>
+    <row r="198" spans="21:23">
+      <c r="U198" s="8"/>
+      <c r="V198" s="8"/>
+      <c r="W198" s="8"/>
+    </row>
+    <row r="199" spans="21:23">
+      <c r="U199" s="8"/>
+      <c r="V199" s="8"/>
+      <c r="W199" s="8"/>
+    </row>
+    <row r="200" spans="21:23">
+      <c r="U200" s="8"/>
+      <c r="V200" s="8"/>
+      <c r="W200" s="8"/>
+    </row>
+    <row r="201" spans="21:23">
+      <c r="U201" s="8"/>
+      <c r="V201" s="8"/>
+      <c r="W201" s="8"/>
+    </row>
+    <row r="202" spans="21:23">
+      <c r="U202" s="8"/>
+      <c r="V202" s="8"/>
+      <c r="W202" s="8"/>
+    </row>
+    <row r="203" spans="21:23">
+      <c r="U203" s="8"/>
+      <c r="V203" s="8"/>
+      <c r="W203" s="8"/>
+    </row>
+    <row r="204" spans="21:23">
+      <c r="U204" s="8"/>
+      <c r="V204" s="8"/>
+      <c r="W204" s="8"/>
+    </row>
+    <row r="205" spans="21:23">
+      <c r="U205" s="8"/>
+      <c r="V205" s="8"/>
+      <c r="W205" s="8"/>
+    </row>
+    <row r="206" spans="21:23">
+      <c r="U206" s="8"/>
+      <c r="V206" s="8"/>
+      <c r="W206" s="8"/>
+    </row>
+    <row r="207" spans="21:23">
+      <c r="U207" s="8"/>
+      <c r="V207" s="8"/>
+      <c r="W207" s="8"/>
+    </row>
+    <row r="208" spans="21:23">
+      <c r="U208" s="8"/>
+      <c r="V208" s="8"/>
+      <c r="W208" s="8"/>
+    </row>
+    <row r="209" spans="21:23">
+      <c r="U209" s="8"/>
+      <c r="V209" s="8"/>
+      <c r="W209" s="8"/>
+    </row>
+    <row r="210" spans="21:23">
+      <c r="U210" s="8"/>
+      <c r="V210" s="8"/>
+      <c r="W210" s="8"/>
+    </row>
+    <row r="211" spans="21:23">
+      <c r="U211" s="8"/>
+      <c r="V211" s="8"/>
+      <c r="W211" s="8"/>
+    </row>
+    <row r="212" spans="21:23">
+      <c r="U212" s="8"/>
+      <c r="V212" s="8"/>
+      <c r="W212" s="8"/>
+    </row>
+    <row r="213" spans="21:23">
+      <c r="U213" s="8"/>
+      <c r="V213" s="8"/>
+      <c r="W213" s="8"/>
+    </row>
+    <row r="214" spans="21:23">
+      <c r="U214" s="8"/>
+      <c r="V214" s="8"/>
+      <c r="W214" s="8"/>
+    </row>
+    <row r="225" spans="21:23">
+      <c r="U225" s="8"/>
+      <c r="V225" s="8"/>
+      <c r="W225" s="8"/>
+    </row>
+    <row r="226" spans="21:23">
+      <c r="U226" s="8"/>
+      <c r="V226" s="8"/>
+      <c r="W226" s="8"/>
+    </row>
+    <row r="227" spans="21:23">
+      <c r="U227" s="8"/>
+      <c r="V227" s="8"/>
+      <c r="W227" s="8"/>
+    </row>
+    <row r="228" spans="21:23">
+      <c r="U228" s="8"/>
+      <c r="V228" s="8"/>
+      <c r="W228" s="8"/>
+    </row>
+    <row r="229" spans="21:23">
+      <c r="U229" s="8"/>
+      <c r="V229" s="8"/>
+      <c r="W229" s="8"/>
+    </row>
+    <row r="230" spans="21:23">
+      <c r="U230" s="8"/>
+      <c r="V230" s="8"/>
+      <c r="W230" s="8"/>
+    </row>
+    <row r="231" spans="21:23">
+      <c r="U231" s="8"/>
+      <c r="V231" s="8"/>
+      <c r="W231" s="8"/>
+    </row>
+    <row r="232" spans="21:23">
+      <c r="U232" s="8"/>
+      <c r="V232" s="8"/>
+      <c r="W232" s="8"/>
+    </row>
+    <row r="233" spans="21:23">
+      <c r="U233" s="8"/>
+      <c r="V233" s="8"/>
+      <c r="W233" s="8"/>
+    </row>
+    <row r="234" spans="21:23">
+      <c r="U234" s="8"/>
+      <c r="V234" s="8"/>
+      <c r="W234" s="8"/>
+    </row>
+    <row r="235" spans="21:23">
+      <c r="U235" s="8"/>
+      <c r="V235" s="8"/>
+      <c r="W235" s="8"/>
+    </row>
+    <row r="236" spans="21:23">
+      <c r="U236" s="8"/>
+      <c r="V236" s="8"/>
+      <c r="W236" s="8"/>
+    </row>
+    <row r="237" spans="21:23">
+      <c r="U237" s="8"/>
+      <c r="V237" s="8"/>
+      <c r="W237" s="8"/>
+    </row>
+    <row r="238" spans="21:23">
+      <c r="U238" s="8"/>
+      <c r="V238" s="8"/>
+      <c r="W238" s="8"/>
+    </row>
+    <row r="239" spans="21:23">
+      <c r="U239" s="8"/>
+      <c r="V239" s="8"/>
+      <c r="W239" s="8"/>
+    </row>
+    <row r="240" spans="21:23">
+      <c r="U240" s="8"/>
+      <c r="V240" s="8"/>
+      <c r="W240" s="8"/>
+    </row>
+    <row r="241" spans="21:23">
+      <c r="U241" s="8"/>
+      <c r="V241" s="8"/>
+      <c r="W241" s="8"/>
+    </row>
+    <row r="242" spans="21:23">
+      <c r="U242" s="8"/>
+      <c r="V242" s="8"/>
+      <c r="W242" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3944,14 +5211,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3959,16 +5226,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="E3" t="s">
         <v>9</v>
       </c>
@@ -3982,7 +5249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -4009,7 +5276,7 @@
         <v>95.420821123013312</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -4036,7 +5303,7 @@
         <v>116.0732967217551</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -4063,7 +5330,7 @@
         <v>134.25592852244921</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -4090,7 +5357,7 @@
         <v>154.0447262494018</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -4117,7 +5384,7 @@
         <v>176.69310271073329</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -4144,7 +5411,7 @@
         <v>200.69190080097081</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -4171,7 +5438,7 @@
         <v>226.41151144353103</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -4198,7 +5465,7 @@
         <v>253.86808638923299</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -4225,7 +5492,7 @@
         <v>284.82819371064102</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -4252,7 +5519,7 @@
         <v>319.49290873548603</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -4279,7 +5546,7 @@
         <v>359.391955818079</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -4306,7 +5573,7 @@
         <v>407.40443950613002</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -4333,7 +5600,7 @@
         <v>462.63517346166896</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -4360,7 +5627,7 @@
         <v>529.80035024901804</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
@@ -4387,7 +5654,7 @@
         <v>608.14725309033997</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
@@ -4414,7 +5681,7 @@
         <v>738.30276348030498</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
         <v>4</v>
       </c>

</xml_diff>